<commit_message>
"static" attributes are now accessible. Setting the tap turn via thei nput file is now also supported.
</commit_message>
<xml_diff>
--- a/mosaik_pypower/test/data/test_case_b.xlsx
+++ b/mosaik_pypower/test/data/test_case_b.xlsx
@@ -1,21 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8200" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Nodes" sheetId="1" r:id="rId1"/>
     <sheet name="Lines" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="29">
   <si>
     <t>Base voltage [kV]</t>
   </si>
@@ -99,6 +104,9 @@
   </si>
   <si>
     <t>Name</t>
+  </si>
+  <si>
+    <t>Tap</t>
   </si>
 </sst>
 </file>
@@ -106,7 +114,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -187,8 +195,8 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -561,18 +569,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK7"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="20" style="1"/>
-    <col min="2" max="2" width="19.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.5703125" style="1"/>
-    <col min="5" max="1025" width="11.42578125" style="1"/>
+    <col min="1" max="1" width="9.1640625" style="1"/>
+    <col min="2" max="2" width="19.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="1025" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -586,7 +593,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -600,7 +607,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -608,7 +615,7 @@
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -619,7 +626,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -630,7 +637,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -641,7 +648,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -655,25 +662,30 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AML8"/>
+  <dimension ref="A1:AMM8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="3" width="9.5703125" style="1" customWidth="1"/>
-    <col min="4" max="6" width="14.28515625" style="1"/>
-    <col min="7" max="7" width="29.7109375" style="1"/>
-    <col min="8" max="1026" width="11.42578125" style="1"/>
+    <col min="1" max="1" width="9.1640625" style="1"/>
+    <col min="2" max="3" width="9.5" style="1" customWidth="1"/>
+    <col min="4" max="1027" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" s="4" t="s">
         <v>27</v>
       </c>
@@ -693,10 +705,13 @@
         <v>20</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
@@ -706,8 +721,9 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2" s="3"/>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
@@ -726,9 +742,12 @@
       <c r="F3" s="1">
         <v>1</v>
       </c>
-      <c r="G3"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G3" s="1">
+        <v>0</v>
+      </c>
+      <c r="H3"/>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" s="3" t="s">
         <v>26</v>
       </c>
@@ -738,8 +757,9 @@
       <c r="E4" s="6"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4" s="3"/>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
         <v>21</v>
       </c>
@@ -758,9 +778,9 @@
       <c r="F5" s="1">
         <v>1</v>
       </c>
-      <c r="G5"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5"/>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
         <v>22</v>
       </c>
@@ -780,7 +800,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
         <v>23</v>
       </c>
@@ -800,7 +820,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
         <v>24</v>
       </c>
@@ -823,5 +843,10 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Present only SI units to the user.
</commit_message>
<xml_diff>
--- a/mosaik_pypower/test/data/test_case_b.xlsx
+++ b/mosaik_pypower/test/data/test_case_b.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8200" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17480"/>
   </bookViews>
   <sheets>
     <sheet name="Nodes" sheetId="1" r:id="rId1"/>
@@ -569,7 +569,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
@@ -674,9 +674,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMM8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>

</xml_diff>